<commit_message>
Updates to matrix based on test updates.
</commit_message>
<xml_diff>
--- a/public/downloads/onc_program_matrix_1_1_0.xlsx
+++ b/public/downloads/onc_program_matrix_1_1_0.xlsx
@@ -24199,7 +24199,7 @@
         <v>ATT-12</v>
       </c>
       <c r="D459" s="158" t="str">
-        <v>Health IT developer demonstrates support for the Patient Demographics Suffix USCDI v1 element by using the Patient.name.suffix FHIR element.</v>
+        <v>Health IT developer demonstrates support for the Patient Demographics Suffix USCDI v1 element.</v>
       </c>
       <c r="E459" s="158" t="str">
         <v xml:space="preserve">ONC certification criteria states that all USCDI v1 data classes and elements need to be supported, including Patient
@@ -24225,7 +24225,7 @@
         <v>ATT-13</v>
       </c>
       <c r="D460" s="158" t="str">
-        <v>Health IT developer demonstrates support for the Patient Demographics Previous Name USCDI v1 element by using the Patient.name.period FHIR element.</v>
+        <v>Health IT developer demonstrates support for the Patient Demographics Previous Name USCDI v1 element.</v>
       </c>
       <c r="E460" s="158" t="str">
         <v xml:space="preserve">ONC certification criteria states that all USCDI v1 data classes and elements need to be supported, including Patient
@@ -24251,7 +24251,7 @@
         <v>ATT-14</v>
       </c>
       <c r="D461" s="158" t="str">
-        <v>Health IT developer demonstrates support for the Allergy and Intolerances Reaction USCDI v1 element by using the AllergyIntolerance.reaction FHIR element.</v>
+        <v>Health IT developer demonstrates support for the Allergy and Intolerances Reaction USCDI v1 element.</v>
       </c>
       <c r="E461" s="158" t="str">
         <v xml:space="preserve">ONC certification criteria states that all USCDI v1 needs to be supported, including Allergies

</xml_diff>